<commit_message>
added updated PR files
</commit_message>
<xml_diff>
--- a/data/p_r_rates/respo_schedule.xlsx
+++ b/data/p_r_rates/respo_schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/moorea_symbiotic_exchange_2023/data/p_r_rates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F21153-F2E9-9C41-BD03-8C855EF8DA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB7A77E-CE02-544C-AF22-8A786CB6ACB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1000" windowWidth="26700" windowHeight="16440" xr2:uid="{5729F46E-A762-7541-B285-883AEFE5FB2E}"/>
+    <workbookView xWindow="1800" yWindow="1340" windowWidth="26700" windowHeight="16440" xr2:uid="{5729F46E-A762-7541-B285-883AEFE5FB2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>Load + Ramp</t>
   </si>
@@ -132,6 +132,24 @@
   </si>
   <si>
     <t xml:space="preserve">Sample 17:30 </t>
+  </si>
+  <si>
+    <t>Prep chambers 11:30</t>
+  </si>
+  <si>
+    <t>Prep chambers 14:00</t>
+  </si>
+  <si>
+    <t>Prep chambers 16:30</t>
+  </si>
+  <si>
+    <t>Rearrange</t>
+  </si>
+  <si>
+    <t>Prep load</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prep load </t>
   </si>
 </sst>
 </file>
@@ -510,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F1FC616-4431-5F46-B60E-95589F590DDB}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -681,6 +699,9 @@
       <c r="E11" s="4">
         <v>0.41666666666666702</v>
       </c>
+      <c r="F11" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="J11" s="4">
         <v>0.41666666666666702</v>
       </c>
@@ -692,8 +713,11 @@
       <c r="E12" s="4">
         <v>0.4375</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="5" t="s">
         <v>0</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="J12" s="4">
         <v>0.4375</v>
@@ -706,7 +730,7 @@
       <c r="E13" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="5" t="s">
         <v>26</v>
       </c>
       <c r="J13" s="4">
@@ -720,6 +744,9 @@
       <c r="E14" s="4">
         <v>0.47916666666666702</v>
       </c>
+      <c r="H14" t="s">
+        <v>32</v>
+      </c>
       <c r="J14" s="4">
         <v>0.47916666666666702</v>
       </c>
@@ -734,7 +761,7 @@
       <c r="E15" s="4">
         <v>0.5</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="2" t="s">
         <v>24</v>
       </c>
       <c r="J15" s="4">
@@ -751,7 +778,10 @@
       <c r="E16" s="4">
         <v>0.52083333333333304</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="G16" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>25</v>
       </c>
       <c r="J16" s="4">
@@ -766,10 +796,13 @@
       <c r="E17" s="4">
         <v>0.54166666666666696</v>
       </c>
+      <c r="F17" t="s">
+        <v>35</v>
+      </c>
       <c r="G17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H17" s="5"/>
+      <c r="H17" s="2"/>
       <c r="J17" s="4">
         <v>0.54166666666666696</v>
       </c>
@@ -801,6 +834,9 @@
       <c r="E19" s="4">
         <v>0.58333333333333304</v>
       </c>
+      <c r="F19" t="s">
+        <v>33</v>
+      </c>
       <c r="J19" s="4">
         <v>0.58333333333333304</v>
       </c>
@@ -832,6 +868,9 @@
       <c r="F21" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="G21" t="s">
+        <v>35</v>
+      </c>
       <c r="J21" s="4">
         <v>0.625</v>
       </c>
@@ -869,6 +908,9 @@
       </c>
       <c r="E24" s="4">
         <v>0.6875</v>
+      </c>
+      <c r="G24" t="s">
+        <v>34</v>
       </c>
       <c r="J24" s="4">
         <v>0.6875</v>

</xml_diff>